<commit_message>
04.02.2020 Mugdho Corporation Sales Details
</commit_message>
<xml_diff>
--- a/2020/January/All Details/04.01.2020/MC Balance Transfer Jan'2020.xlsx
+++ b/2020/January/All Details/04.01.2020/MC Balance Transfer Jan'2020.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\January\All Details\04.01.2020\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965CC91F-971A-4633-9283-83C3F6701C59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="598"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Oct'19 Sales+Cost+Bank+Balanch" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -22,12 +28,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>LENOVO</author>
   </authors>
   <commentList>
-    <comment ref="C41" authorId="0">
+    <comment ref="C41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C42" authorId="0">
+    <comment ref="C42" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -272,26 +278,23 @@
     <t>01.01.2020</t>
   </si>
   <si>
-    <t>Desh</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
     <t>02.01.2020</t>
   </si>
   <si>
-    <t>S.A Mobile Mart</t>
+    <t>04.01.2020</t>
   </si>
   <si>
-    <t>Maa Telecom</t>
+    <t>04.02.2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1200,7 +1203,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1212,7 +1215,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1235,14 +1238,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1302,7 +1305,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1334,9 +1337,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1368,6 +1389,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1543,19 +1582,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BI232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="C101" sqref="C101"/>
+      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="4" customWidth="1"/>
@@ -1576,7 +1615,7 @@
     <col min="40" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="15.75" customHeight="1">
+    <row r="1" spans="1:61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="148" t="s">
         <v>22</v>
       </c>
@@ -1636,7 +1675,7 @@
       <c r="BH1" s="7"/>
       <c r="BI1" s="7"/>
     </row>
-    <row r="2" spans="1:61" ht="12.75" hidden="1" customHeight="1">
+    <row r="2" spans="1:61" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="150" t="s">
         <v>11</v>
       </c>
@@ -1699,7 +1738,7 @@
       <c r="BH2" s="7"/>
       <c r="BI2" s="7"/>
     </row>
-    <row r="3" spans="1:61" ht="21" hidden="1" customHeight="1">
+    <row r="3" spans="1:61" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="151" t="s">
         <v>13</v>
       </c>
@@ -1759,7 +1798,7 @@
       <c r="BH3" s="7"/>
       <c r="BI3" s="7"/>
     </row>
-    <row r="4" spans="1:61" ht="17.25" customHeight="1" thickBot="1">
+    <row r="4" spans="1:61" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="163" t="s">
         <v>19</v>
       </c>
@@ -1820,7 +1859,7 @@
       <c r="BH4" s="7"/>
       <c r="BI4" s="7"/>
     </row>
-    <row r="5" spans="1:61" ht="12.6" customHeight="1" thickTop="1" thickBot="1">
+    <row r="5" spans="1:61" ht="12.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="145" t="s">
         <v>0</v>
       </c>
@@ -1895,7 +1934,7 @@
       <c r="BH5" s="7"/>
       <c r="BI5" s="7"/>
     </row>
-    <row r="6" spans="1:61" ht="12.6" customHeight="1">
+    <row r="6" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="143" t="s">
         <v>61</v>
       </c>
@@ -1975,9 +2014,9 @@
       <c r="BH6" s="7"/>
       <c r="BI6" s="7"/>
     </row>
-    <row r="7" spans="1:61" ht="12.6" customHeight="1">
+    <row r="7" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2">
         <v>208340</v>
@@ -2001,7 +2040,7 @@
         <v>450</v>
       </c>
       <c r="J7" s="43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K7" s="128"/>
       <c r="L7" s="19"/>
@@ -2055,22 +2094,34 @@
       <c r="BH7" s="7"/>
       <c r="BI7" s="7"/>
     </row>
-    <row r="8" spans="1:61" ht="12.6" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+    <row r="8" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="2">
+        <v>380365</v>
+      </c>
+      <c r="C8" s="2">
+        <v>329020</v>
+      </c>
+      <c r="D8" s="2">
+        <v>608</v>
+      </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>329628</v>
       </c>
       <c r="F8" s="135"/>
       <c r="G8" s="112"/>
       <c r="H8" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="64"/>
-      <c r="J8" s="43"/>
+      <c r="I8" s="64">
+        <v>2010</v>
+      </c>
+      <c r="J8" s="43" t="s">
+        <v>64</v>
+      </c>
       <c r="K8" s="128"/>
       <c r="L8" s="19"/>
       <c r="M8" s="3"/>
@@ -2123,7 +2174,7 @@
       <c r="BH8" s="7"/>
       <c r="BI8" s="7"/>
     </row>
-    <row r="9" spans="1:61" ht="12.6" customHeight="1">
+    <row r="9" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2191,7 +2242,7 @@
       <c r="BH9" s="7"/>
       <c r="BI9" s="7"/>
     </row>
-    <row r="10" spans="1:61" ht="12" customHeight="1">
+    <row r="10" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2259,7 +2310,7 @@
       <c r="BH10" s="7"/>
       <c r="BI10" s="7"/>
     </row>
-    <row r="11" spans="1:61" ht="12.6" customHeight="1">
+    <row r="11" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2327,7 +2378,7 @@
       <c r="BH11" s="7"/>
       <c r="BI11" s="7"/>
     </row>
-    <row r="12" spans="1:61" ht="12.6" customHeight="1">
+    <row r="12" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2395,7 +2446,7 @@
       <c r="BH12" s="7"/>
       <c r="BI12" s="7"/>
     </row>
-    <row r="13" spans="1:61" ht="12.6" customHeight="1">
+    <row r="13" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2463,7 +2514,7 @@
       <c r="BH13" s="7"/>
       <c r="BI13" s="7"/>
     </row>
-    <row r="14" spans="1:61" ht="12.6" customHeight="1">
+    <row r="14" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2531,7 +2582,7 @@
       <c r="BH14" s="7"/>
       <c r="BI14" s="7"/>
     </row>
-    <row r="15" spans="1:61" ht="12.6" customHeight="1">
+    <row r="15" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2599,7 +2650,7 @@
       <c r="BH15" s="7"/>
       <c r="BI15" s="7"/>
     </row>
-    <row r="16" spans="1:61" ht="12.6" customHeight="1">
+    <row r="16" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2667,7 +2718,7 @@
       <c r="BH16" s="7"/>
       <c r="BI16" s="7"/>
     </row>
-    <row r="17" spans="1:61" ht="12.6" customHeight="1">
+    <row r="17" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2735,7 +2786,7 @@
       <c r="BH17" s="7"/>
       <c r="BI17" s="7"/>
     </row>
-    <row r="18" spans="1:61" ht="12.6" customHeight="1">
+    <row r="18" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2803,7 +2854,7 @@
       <c r="BH18" s="7"/>
       <c r="BI18" s="7"/>
     </row>
-    <row r="19" spans="1:61" ht="12.6" customHeight="1">
+    <row r="19" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2871,7 +2922,7 @@
       <c r="BH19" s="7"/>
       <c r="BI19" s="7"/>
     </row>
-    <row r="20" spans="1:61" ht="12.6" customHeight="1">
+    <row r="20" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2939,7 +2990,7 @@
       <c r="BH20" s="7"/>
       <c r="BI20" s="7"/>
     </row>
-    <row r="21" spans="1:61" ht="12.6" customHeight="1">
+    <row r="21" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3007,7 +3058,7 @@
       <c r="BH21" s="7"/>
       <c r="BI21" s="7"/>
     </row>
-    <row r="22" spans="1:61" ht="12.6" customHeight="1">
+    <row r="22" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3075,7 +3126,7 @@
       <c r="BH22" s="7"/>
       <c r="BI22" s="7"/>
     </row>
-    <row r="23" spans="1:61" ht="12.6" customHeight="1">
+    <row r="23" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3143,7 +3194,7 @@
       <c r="BH23" s="7"/>
       <c r="BI23" s="7"/>
     </row>
-    <row r="24" spans="1:61" ht="12.6" customHeight="1">
+    <row r="24" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3211,7 +3262,7 @@
       <c r="BH24" s="7"/>
       <c r="BI24" s="7"/>
     </row>
-    <row r="25" spans="1:61" ht="12.6" customHeight="1">
+    <row r="25" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3279,7 +3330,7 @@
       <c r="BH25" s="7"/>
       <c r="BI25" s="7"/>
     </row>
-    <row r="26" spans="1:61" ht="12.6" customHeight="1">
+    <row r="26" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3347,7 +3398,7 @@
       <c r="BH26" s="7"/>
       <c r="BI26" s="7"/>
     </row>
-    <row r="27" spans="1:61" ht="12.6" customHeight="1">
+    <row r="27" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3415,7 +3466,7 @@
       <c r="BH27" s="7"/>
       <c r="BI27" s="7"/>
     </row>
-    <row r="28" spans="1:61" ht="12.6" customHeight="1">
+    <row r="28" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3483,7 +3534,7 @@
       <c r="BH28" s="7"/>
       <c r="BI28" s="7"/>
     </row>
-    <row r="29" spans="1:61" ht="12.6" customHeight="1">
+    <row r="29" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3551,7 +3602,7 @@
       <c r="BH29" s="7"/>
       <c r="BI29" s="7"/>
     </row>
-    <row r="30" spans="1:61" ht="12.6" customHeight="1">
+    <row r="30" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3619,7 +3670,7 @@
       <c r="BH30" s="7"/>
       <c r="BI30" s="7"/>
     </row>
-    <row r="31" spans="1:61" ht="12.6" customHeight="1">
+    <row r="31" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3687,7 +3738,7 @@
       <c r="BH31" s="7"/>
       <c r="BI31" s="7"/>
     </row>
-    <row r="32" spans="1:61" ht="12.6" customHeight="1">
+    <row r="32" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3755,7 +3806,7 @@
       <c r="BH32" s="7"/>
       <c r="BI32" s="7"/>
     </row>
-    <row r="33" spans="1:61" ht="12.6" customHeight="1">
+    <row r="33" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3821,29 +3872,29 @@
       <c r="BH33" s="7"/>
       <c r="BI33" s="7"/>
     </row>
-    <row r="34" spans="1:61">
+    <row r="34" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="2">
         <f>SUM(B6:B33)</f>
-        <v>482480</v>
+        <v>862845</v>
       </c>
       <c r="C34" s="2">
         <f>SUM(C6:C33)</f>
-        <v>538540</v>
+        <v>867560</v>
       </c>
       <c r="D34" s="2">
         <f>SUM(D6:D33)</f>
-        <v>1620</v>
+        <v>2228</v>
       </c>
       <c r="E34" s="2">
         <f>SUM(E6:E33)</f>
-        <v>540160</v>
+        <v>869788</v>
       </c>
       <c r="F34" s="94">
         <f>B34-E34</f>
-        <v>-57680</v>
+        <v>-6943</v>
       </c>
       <c r="G34" s="114"/>
       <c r="H34" s="124"/>
@@ -3901,7 +3952,7 @@
       <c r="BH34" s="7"/>
       <c r="BI34" s="7"/>
     </row>
-    <row r="35" spans="1:61" ht="12.6" customHeight="1">
+    <row r="35" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -3964,7 +4015,7 @@
       <c r="BH35" s="7"/>
       <c r="BI35" s="7"/>
     </row>
-    <row r="36" spans="1:61" ht="12.6" customHeight="1" thickBot="1">
+    <row r="36" spans="1:61" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="164" t="s">
         <v>7</v>
       </c>
@@ -4029,7 +4080,7 @@
       <c r="BH36" s="7"/>
       <c r="BI36" s="7"/>
     </row>
-    <row r="37" spans="1:61" ht="12.6" customHeight="1">
+    <row r="37" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="38" t="s">
         <v>8</v>
       </c>
@@ -4106,7 +4157,7 @@
       <c r="BH37" s="7"/>
       <c r="BI37" s="7"/>
     </row>
-    <row r="38" spans="1:61" ht="12.6" customHeight="1">
+    <row r="38" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>30</v>
       </c>
@@ -4177,7 +4228,7 @@
       <c r="BH38" s="7"/>
       <c r="BI38" s="7"/>
     </row>
-    <row r="39" spans="1:61" ht="12.6" customHeight="1">
+    <row r="39" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>51</v>
       </c>
@@ -4248,7 +4299,7 @@
       <c r="BH39" s="7"/>
       <c r="BI39" s="7"/>
     </row>
-    <row r="40" spans="1:61" ht="12.6" customHeight="1">
+    <row r="40" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>54</v>
       </c>
@@ -4319,7 +4370,7 @@
       <c r="BH40" s="7"/>
       <c r="BI40" s="7"/>
     </row>
-    <row r="41" spans="1:61" ht="12.6" customHeight="1">
+    <row r="41" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>42</v>
       </c>
@@ -4390,7 +4441,7 @@
       <c r="BH41" s="7"/>
       <c r="BI41" s="7"/>
     </row>
-    <row r="42" spans="1:61" ht="12.6" customHeight="1">
+    <row r="42" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="40" t="s">
         <v>36</v>
       </c>
@@ -4459,7 +4510,7 @@
       <c r="BH42" s="7"/>
       <c r="BI42" s="7"/>
     </row>
-    <row r="43" spans="1:61" ht="12.6" customHeight="1">
+    <row r="43" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="47" t="s">
         <v>34</v>
       </c>
@@ -4529,7 +4580,7 @@
       <c r="BH43" s="7"/>
       <c r="BI43" s="7"/>
     </row>
-    <row r="44" spans="1:61" ht="12.6" customHeight="1">
+    <row r="44" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
       <c r="B44" s="1"/>
       <c r="C44" s="2"/>
@@ -4596,11 +4647,11 @@
       <c r="BH44" s="7"/>
       <c r="BI44" s="7"/>
     </row>
-    <row r="45" spans="1:61" ht="12.6" customHeight="1" thickBot="1">
+    <row r="45" spans="1:61" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="73"/>
       <c r="B45" s="74"/>
       <c r="C45" s="75">
-        <v>10323</v>
+        <v>435</v>
       </c>
       <c r="D45" s="76"/>
       <c r="E45" s="3"/>
@@ -4659,7 +4710,7 @@
       <c r="BH45" s="7"/>
       <c r="BI45" s="7"/>
     </row>
-    <row r="46" spans="1:61" ht="12" customHeight="1" thickTop="1" thickBot="1">
+    <row r="46" spans="1:61" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="69"/>
       <c r="B46" s="70"/>
       <c r="C46" s="71"/>
@@ -4720,7 +4771,7 @@
       <c r="BH46" s="7"/>
       <c r="BI46" s="7"/>
     </row>
-    <row r="47" spans="1:61" ht="12" customHeight="1" thickTop="1">
+    <row r="47" spans="1:61" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A47" s="101" t="s">
         <v>24</v>
       </c>
@@ -4787,7 +4838,7 @@
       <c r="BH47" s="7"/>
       <c r="BI47" s="7"/>
     </row>
-    <row r="48" spans="1:61" ht="12.75" customHeight="1">
+    <row r="48" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="104" t="s">
         <v>25</v>
       </c>
@@ -4799,7 +4850,7 @@
         <v>23</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
@@ -4856,7 +4907,7 @@
       <c r="BH48" s="7"/>
       <c r="BI48" s="7"/>
     </row>
-    <row r="49" spans="1:61" ht="12" customHeight="1">
+    <row r="49" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="105" t="s">
         <v>26</v>
       </c>
@@ -4923,7 +4974,7 @@
       <c r="BH49" s="7"/>
       <c r="BI49" s="7"/>
     </row>
-    <row r="50" spans="1:61">
+    <row r="50" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A50" s="100" t="s">
         <v>27</v>
       </c>
@@ -4932,7 +4983,7 @@
         <v>99210</v>
       </c>
       <c r="D50" s="99" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="12"/>
@@ -4990,7 +5041,7 @@
       <c r="BH50" s="7"/>
       <c r="BI50" s="7"/>
     </row>
-    <row r="51" spans="1:61" ht="11.25" customHeight="1">
+    <row r="51" spans="1:61" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="105" t="s">
         <v>32</v>
       </c>
@@ -5057,16 +5108,16 @@
       <c r="BH51" s="7"/>
       <c r="BI51" s="7"/>
     </row>
-    <row r="52" spans="1:61" ht="12" customHeight="1">
+    <row r="52" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="105" t="s">
         <v>31</v>
       </c>
       <c r="B52" s="43"/>
       <c r="C52" s="98">
-        <v>199545</v>
+        <v>285020</v>
       </c>
       <c r="D52" s="99" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="43"/>
@@ -5126,7 +5177,7 @@
       <c r="BH52" s="7"/>
       <c r="BI52" s="7"/>
     </row>
-    <row r="53" spans="1:61" ht="12" customHeight="1">
+    <row r="53" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="105" t="s">
         <v>37</v>
       </c>
@@ -5135,7 +5186,7 @@
         <v>184000</v>
       </c>
       <c r="D53" s="102" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="12"/>
@@ -5195,16 +5246,16 @@
       <c r="BH53" s="7"/>
       <c r="BI53" s="7"/>
     </row>
-    <row r="54" spans="1:61" ht="12" customHeight="1">
+    <row r="54" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="100" t="s">
         <v>38</v>
       </c>
       <c r="B54" s="97"/>
       <c r="C54" s="106">
-        <v>20000</v>
+        <v>26000</v>
       </c>
       <c r="D54" s="99" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="64"/>
@@ -5264,7 +5315,7 @@
       <c r="BH54" s="7"/>
       <c r="BI54" s="7"/>
     </row>
-    <row r="55" spans="1:61" ht="12" customHeight="1">
+    <row r="55" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="100" t="s">
         <v>39</v>
       </c>
@@ -5333,7 +5384,7 @@
       <c r="BH55" s="7"/>
       <c r="BI55" s="7"/>
     </row>
-    <row r="56" spans="1:61" ht="12" customHeight="1">
+    <row r="56" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="100" t="s">
         <v>45</v>
       </c>
@@ -5404,13 +5455,13 @@
       <c r="BH56" s="7"/>
       <c r="BI56" s="7"/>
     </row>
-    <row r="57" spans="1:61" ht="12" customHeight="1">
+    <row r="57" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="100" t="s">
         <v>46</v>
       </c>
       <c r="B57" s="43"/>
       <c r="C57" s="98">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D57" s="97" t="s">
         <v>64</v>
@@ -5473,17 +5524,11 @@
       <c r="BH57" s="7"/>
       <c r="BI57" s="7"/>
     </row>
-    <row r="58" spans="1:61" ht="12" customHeight="1">
-      <c r="A58" s="100" t="s">
-        <v>62</v>
-      </c>
+    <row r="58" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="100"/>
       <c r="B58" s="43"/>
-      <c r="C58" s="98">
-        <v>4350</v>
-      </c>
-      <c r="D58" s="107" t="s">
-        <v>64</v>
-      </c>
+      <c r="C58" s="98"/>
+      <c r="D58" s="107"/>
       <c r="E58" s="3"/>
       <c r="F58" s="43"/>
       <c r="G58" s="12"/>
@@ -5542,17 +5587,11 @@
       <c r="BH58" s="7"/>
       <c r="BI58" s="7"/>
     </row>
-    <row r="59" spans="1:61" ht="12" customHeight="1">
-      <c r="A59" s="100" t="s">
-        <v>65</v>
-      </c>
+    <row r="59" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="100"/>
       <c r="B59" s="43"/>
-      <c r="C59" s="98">
-        <v>5000</v>
-      </c>
-      <c r="D59" s="107" t="s">
-        <v>64</v>
-      </c>
+      <c r="C59" s="98"/>
+      <c r="D59" s="107"/>
       <c r="E59" s="3"/>
       <c r="F59" s="64"/>
       <c r="G59" s="12"/>
@@ -5611,17 +5650,11 @@
       <c r="BH59" s="7"/>
       <c r="BI59" s="7"/>
     </row>
-    <row r="60" spans="1:61" ht="12" customHeight="1">
-      <c r="A60" s="100" t="s">
-        <v>66</v>
-      </c>
+    <row r="60" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="100"/>
       <c r="B60" s="43"/>
-      <c r="C60" s="98">
-        <v>1500</v>
-      </c>
-      <c r="D60" s="107" t="s">
-        <v>64</v>
-      </c>
+      <c r="C60" s="98"/>
+      <c r="D60" s="107"/>
       <c r="E60" s="3"/>
       <c r="F60" s="43"/>
       <c r="G60" s="12"/>
@@ -5680,7 +5713,7 @@
       <c r="BH60" s="7"/>
       <c r="BI60" s="7"/>
     </row>
-    <row r="61" spans="1:61" ht="12" customHeight="1">
+    <row r="61" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="105"/>
       <c r="B61" s="43"/>
       <c r="C61" s="98"/>
@@ -5743,7 +5776,7 @@
       <c r="BH61" s="7"/>
       <c r="BI61" s="7"/>
     </row>
-    <row r="62" spans="1:61" ht="12" customHeight="1">
+    <row r="62" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="100"/>
       <c r="B62" s="43"/>
       <c r="C62" s="98"/>
@@ -5806,11 +5839,13 @@
       <c r="BH62" s="7"/>
       <c r="BI62" s="7"/>
     </row>
-    <row r="63" spans="1:61" ht="12.75" customHeight="1">
+    <row r="63" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="100"/>
       <c r="B63" s="43"/>
       <c r="C63" s="98"/>
-      <c r="D63" s="99"/>
+      <c r="D63" s="99" t="s">
+        <v>62</v>
+      </c>
       <c r="E63" s="3"/>
       <c r="F63" s="160" t="s">
         <v>28</v>
@@ -5877,7 +5912,7 @@
       <c r="BH63" s="7"/>
       <c r="BI63" s="7"/>
     </row>
-    <row r="64" spans="1:61" ht="12.75" customHeight="1">
+    <row r="64" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="100"/>
       <c r="B64" s="43"/>
       <c r="C64" s="98"/>
@@ -5943,7 +5978,7 @@
       <c r="BH64" s="7"/>
       <c r="BI64" s="7"/>
     </row>
-    <row r="65" spans="1:61" ht="12.75" customHeight="1">
+    <row r="65" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="105"/>
       <c r="B65" s="43"/>
       <c r="C65" s="98"/>
@@ -6009,7 +6044,7 @@
       <c r="BH65" s="7"/>
       <c r="BI65" s="7"/>
     </row>
-    <row r="66" spans="1:61" ht="12.75" customHeight="1">
+    <row r="66" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="100"/>
       <c r="B66" s="43"/>
       <c r="C66" s="98"/>
@@ -6083,7 +6118,7 @@
       <c r="BH66" s="7"/>
       <c r="BI66" s="7"/>
     </row>
-    <row r="67" spans="1:61" ht="12.75" customHeight="1">
+    <row r="67" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="100"/>
       <c r="B67" s="43"/>
       <c r="C67" s="98"/>
@@ -6157,7 +6192,7 @@
       <c r="BH67" s="7"/>
       <c r="BI67" s="7"/>
     </row>
-    <row r="68" spans="1:61" ht="12.75" customHeight="1">
+    <row r="68" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="105"/>
       <c r="B68" s="43"/>
       <c r="C68" s="98"/>
@@ -6231,7 +6266,7 @@
       <c r="BH68" s="7"/>
       <c r="BI68" s="7"/>
     </row>
-    <row r="69" spans="1:61" ht="12.75" customHeight="1">
+    <row r="69" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="105"/>
       <c r="B69" s="43"/>
       <c r="C69" s="98"/>
@@ -6305,7 +6340,7 @@
       <c r="BH69" s="7"/>
       <c r="BI69" s="7"/>
     </row>
-    <row r="70" spans="1:61" ht="12.75" customHeight="1">
+    <row r="70" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="100"/>
       <c r="B70" s="43"/>
       <c r="C70" s="98"/>
@@ -6379,7 +6414,7 @@
       <c r="BH70" s="7"/>
       <c r="BI70" s="7"/>
     </row>
-    <row r="71" spans="1:61" ht="12.75" customHeight="1">
+    <row r="71" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="100"/>
       <c r="B71" s="43"/>
       <c r="C71" s="98"/>
@@ -6453,7 +6488,7 @@
       <c r="BH71" s="7"/>
       <c r="BI71" s="7"/>
     </row>
-    <row r="72" spans="1:61" ht="12.75" customHeight="1">
+    <row r="72" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="105"/>
       <c r="B72" s="43"/>
       <c r="C72" s="98"/>
@@ -6527,7 +6562,7 @@
       <c r="BH72" s="7"/>
       <c r="BI72" s="7"/>
     </row>
-    <row r="73" spans="1:61" ht="12.75" customHeight="1">
+    <row r="73" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="100"/>
       <c r="B73" s="43"/>
       <c r="C73" s="98"/>
@@ -6601,7 +6636,7 @@
       <c r="BH73" s="7"/>
       <c r="BI73" s="7"/>
     </row>
-    <row r="74" spans="1:61" ht="12.75" customHeight="1">
+    <row r="74" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="100"/>
       <c r="B74" s="43"/>
       <c r="C74" s="98"/>
@@ -6675,7 +6710,7 @@
       <c r="BH74" s="7"/>
       <c r="BI74" s="7"/>
     </row>
-    <row r="75" spans="1:61" ht="12.75" customHeight="1">
+    <row r="75" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="100"/>
       <c r="B75" s="43"/>
       <c r="C75" s="98"/>
@@ -6749,7 +6784,7 @@
       <c r="BH75" s="7"/>
       <c r="BI75" s="7"/>
     </row>
-    <row r="76" spans="1:61" ht="12.75" customHeight="1">
+    <row r="76" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="100"/>
       <c r="B76" s="43"/>
       <c r="C76" s="98"/>
@@ -6823,7 +6858,7 @@
       <c r="BH76" s="7"/>
       <c r="BI76" s="7"/>
     </row>
-    <row r="77" spans="1:61" ht="12.75" customHeight="1">
+    <row r="77" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="100"/>
       <c r="B77" s="43"/>
       <c r="C77" s="98"/>
@@ -6897,7 +6932,7 @@
       <c r="BH77" s="7"/>
       <c r="BI77" s="7"/>
     </row>
-    <row r="78" spans="1:61" ht="12.75" customHeight="1">
+    <row r="78" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="105"/>
       <c r="B78" s="43"/>
       <c r="C78" s="98"/>
@@ -6973,7 +7008,7 @@
       <c r="BH78" s="7"/>
       <c r="BI78" s="7"/>
     </row>
-    <row r="79" spans="1:61" ht="12.75" customHeight="1">
+    <row r="79" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="100"/>
       <c r="B79" s="43"/>
       <c r="C79" s="98"/>
@@ -7049,7 +7084,7 @@
       <c r="BH79" s="7"/>
       <c r="BI79" s="7"/>
     </row>
-    <row r="80" spans="1:61" ht="12.75" customHeight="1">
+    <row r="80" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="100"/>
       <c r="B80" s="43"/>
       <c r="C80" s="98"/>
@@ -7125,7 +7160,7 @@
       <c r="BH80" s="7"/>
       <c r="BI80" s="7"/>
     </row>
-    <row r="81" spans="1:61" ht="12.75" customHeight="1">
+    <row r="81" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="100"/>
       <c r="B81" s="43"/>
       <c r="C81" s="98"/>
@@ -7201,7 +7236,7 @@
       <c r="BH81" s="7"/>
       <c r="BI81" s="7"/>
     </row>
-    <row r="82" spans="1:61" ht="12.75" customHeight="1">
+    <row r="82" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="100"/>
       <c r="B82" s="43"/>
       <c r="C82" s="98"/>
@@ -7275,7 +7310,7 @@
       <c r="BH82" s="7"/>
       <c r="BI82" s="7"/>
     </row>
-    <row r="83" spans="1:61" ht="12.75" customHeight="1">
+    <row r="83" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="100"/>
       <c r="B83" s="43"/>
       <c r="C83" s="98"/>
@@ -7351,7 +7386,7 @@
       <c r="BH83" s="7"/>
       <c r="BI83" s="7"/>
     </row>
-    <row r="84" spans="1:61" ht="12.75" customHeight="1">
+    <row r="84" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="105"/>
       <c r="B84" s="99"/>
       <c r="C84" s="98"/>
@@ -7425,7 +7460,7 @@
       <c r="BH84" s="7"/>
       <c r="BI84" s="7"/>
     </row>
-    <row r="85" spans="1:61" ht="12.75" customHeight="1">
+    <row r="85" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="100"/>
       <c r="B85" s="43"/>
       <c r="C85" s="98"/>
@@ -7499,7 +7534,7 @@
       <c r="BH85" s="7"/>
       <c r="BI85" s="7"/>
     </row>
-    <row r="86" spans="1:61" ht="12.75" customHeight="1">
+    <row r="86" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="100"/>
       <c r="B86" s="43"/>
       <c r="C86" s="98"/>
@@ -7569,7 +7604,7 @@
       <c r="BH86" s="7"/>
       <c r="BI86" s="7"/>
     </row>
-    <row r="87" spans="1:61" ht="12.75" customHeight="1">
+    <row r="87" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="100"/>
       <c r="B87" s="43"/>
       <c r="C87" s="98"/>
@@ -7635,7 +7670,7 @@
       <c r="BH87" s="7"/>
       <c r="BI87" s="7"/>
     </row>
-    <row r="88" spans="1:61" ht="12.75" customHeight="1">
+    <row r="88" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="100"/>
       <c r="B88" s="43"/>
       <c r="C88" s="98"/>
@@ -7701,7 +7736,7 @@
       <c r="BH88" s="7"/>
       <c r="BI88" s="7"/>
     </row>
-    <row r="89" spans="1:61" ht="12.75" customHeight="1">
+    <row r="89" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="105"/>
       <c r="B89" s="43"/>
       <c r="C89" s="98"/>
@@ -7767,7 +7802,7 @@
       <c r="BH89" s="7"/>
       <c r="BI89" s="7"/>
     </row>
-    <row r="90" spans="1:61" ht="12.75" customHeight="1">
+    <row r="90" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="100"/>
       <c r="B90" s="43"/>
       <c r="C90" s="98"/>
@@ -7833,7 +7868,7 @@
       <c r="BH90" s="7"/>
       <c r="BI90" s="7"/>
     </row>
-    <row r="91" spans="1:61" ht="12.6" customHeight="1">
+    <row r="91" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="100"/>
       <c r="B91" s="43"/>
       <c r="C91" s="98"/>
@@ -7899,7 +7934,7 @@
       <c r="BH91" s="7"/>
       <c r="BI91" s="7"/>
     </row>
-    <row r="92" spans="1:61" ht="12.75" customHeight="1">
+    <row r="92" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="100"/>
       <c r="B92" s="108"/>
       <c r="C92" s="106"/>
@@ -7965,7 +8000,7 @@
       <c r="BH92" s="7"/>
       <c r="BI92" s="7"/>
     </row>
-    <row r="93" spans="1:61">
+    <row r="93" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A93" s="100"/>
       <c r="B93" s="97"/>
       <c r="C93" s="98"/>
@@ -8030,7 +8065,7 @@
       <c r="BH93" s="7"/>
       <c r="BI93" s="7"/>
     </row>
-    <row r="94" spans="1:61" ht="14.25" customHeight="1">
+    <row r="94" spans="1:61" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="100"/>
       <c r="B94" s="108"/>
       <c r="C94" s="98"/>
@@ -8095,7 +8130,7 @@
       <c r="BH94" s="7"/>
       <c r="BI94" s="7"/>
     </row>
-    <row r="95" spans="1:61" ht="14.25" customHeight="1">
+    <row r="95" spans="1:61" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="105"/>
       <c r="B95" s="99"/>
       <c r="C95" s="98"/>
@@ -8160,7 +8195,7 @@
       <c r="BH95" s="7"/>
       <c r="BI95" s="7"/>
     </row>
-    <row r="96" spans="1:61" ht="14.25" customHeight="1">
+    <row r="96" spans="1:61" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="100"/>
       <c r="B96" s="97"/>
       <c r="C96" s="98"/>
@@ -8225,7 +8260,7 @@
       <c r="BH96" s="7"/>
       <c r="BI96" s="7"/>
     </row>
-    <row r="97" spans="1:61">
+    <row r="97" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A97" s="118" t="s">
         <v>48</v>
       </c>
@@ -8296,7 +8331,7 @@
       <c r="BH97" s="7"/>
       <c r="BI97" s="7"/>
     </row>
-    <row r="98" spans="1:61">
+    <row r="98" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A98" s="118"/>
       <c r="B98" s="119"/>
       <c r="C98" s="120"/>
@@ -8361,14 +8396,14 @@
       <c r="BH98" s="7"/>
       <c r="BI98" s="7"/>
     </row>
-    <row r="99" spans="1:61">
+    <row r="99" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A99" s="158" t="s">
         <v>16</v>
       </c>
       <c r="B99" s="159"/>
       <c r="C99" s="45">
         <f>SUM(C38:C98)</f>
-        <v>1420530</v>
+        <v>1471267</v>
       </c>
       <c r="D99" s="41"/>
       <c r="F99" s="23"/>
@@ -8431,7 +8466,7 @@
       <c r="BH99" s="7"/>
       <c r="BI99" s="7"/>
     </row>
-    <row r="100" spans="1:61">
+    <row r="100" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A100" s="36"/>
       <c r="B100" s="37"/>
       <c r="C100" s="46"/>
@@ -8496,14 +8531,14 @@
       <c r="BH100" s="7"/>
       <c r="BI100" s="7"/>
     </row>
-    <row r="101" spans="1:61">
+    <row r="101" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A101" s="156" t="s">
         <v>18</v>
       </c>
       <c r="B101" s="157"/>
       <c r="C101" s="42">
         <f>C99+L122</f>
-        <v>1420530</v>
+        <v>1471267</v>
       </c>
       <c r="D101" s="26"/>
       <c r="F101" s="24"/>
@@ -8566,7 +8601,7 @@
       <c r="BH101" s="7"/>
       <c r="BI101" s="7"/>
     </row>
-    <row r="102" spans="1:61">
+    <row r="102" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A102" s="59"/>
       <c r="B102" s="7"/>
       <c r="C102" s="60"/>
@@ -8631,7 +8666,7 @@
       <c r="BH102" s="7"/>
       <c r="BI102" s="7"/>
     </row>
-    <row r="103" spans="1:61">
+    <row r="103" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A103" s="59"/>
       <c r="B103" s="7"/>
       <c r="D103" s="60"/>
@@ -8695,7 +8730,7 @@
       <c r="BH103" s="7"/>
       <c r="BI103" s="7"/>
     </row>
-    <row r="104" spans="1:61">
+    <row r="104" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A104" s="61"/>
       <c r="B104" s="61"/>
       <c r="C104" s="60"/>
@@ -8760,7 +8795,7 @@
       <c r="BH104" s="7"/>
       <c r="BI104" s="7"/>
     </row>
-    <row r="105" spans="1:61">
+    <row r="105" spans="1:61" x14ac:dyDescent="0.2">
       <c r="C105" s="33"/>
       <c r="F105" s="24"/>
       <c r="G105" s="13"/>
@@ -8822,7 +8857,7 @@
       <c r="BH105" s="7"/>
       <c r="BI105" s="7"/>
     </row>
-    <row r="106" spans="1:61">
+    <row r="106" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A106" s="54"/>
       <c r="B106" s="55"/>
       <c r="C106" s="56"/>
@@ -8887,7 +8922,7 @@
       <c r="BH106" s="7"/>
       <c r="BI106" s="7"/>
     </row>
-    <row r="107" spans="1:61">
+    <row r="107" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A107" s="54"/>
       <c r="B107" s="55"/>
       <c r="C107" s="56"/>
@@ -8952,7 +8987,7 @@
       <c r="BH107" s="7"/>
       <c r="BI107" s="7"/>
     </row>
-    <row r="108" spans="1:61">
+    <row r="108" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A108" s="55"/>
       <c r="B108" s="58"/>
       <c r="C108" s="56"/>
@@ -9017,7 +9052,7 @@
       <c r="BH108" s="7"/>
       <c r="BI108" s="7"/>
     </row>
-    <row r="109" spans="1:61">
+    <row r="109" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A109" s="54"/>
       <c r="B109" s="55"/>
       <c r="C109" s="56"/>
@@ -9082,7 +9117,7 @@
       <c r="BH109" s="7"/>
       <c r="BI109" s="7"/>
     </row>
-    <row r="110" spans="1:61">
+    <row r="110" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A110" s="50"/>
       <c r="B110" s="51"/>
       <c r="C110" s="52"/>
@@ -9147,7 +9182,7 @@
       <c r="BH110" s="7"/>
       <c r="BI110" s="7"/>
     </row>
-    <row r="111" spans="1:61">
+    <row r="111" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A111" s="50"/>
       <c r="B111" s="51"/>
       <c r="C111" s="52"/>
@@ -9212,7 +9247,7 @@
       <c r="BH111" s="7"/>
       <c r="BI111" s="7"/>
     </row>
-    <row r="112" spans="1:61">
+    <row r="112" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A112" s="50"/>
       <c r="B112" s="51"/>
       <c r="C112" s="52"/>
@@ -9277,7 +9312,7 @@
       <c r="BH112" s="7"/>
       <c r="BI112" s="7"/>
     </row>
-    <row r="113" spans="1:61">
+    <row r="113" spans="1:61" x14ac:dyDescent="0.2">
       <c r="C113" s="33"/>
       <c r="F113" s="23"/>
       <c r="G113" s="13"/>
@@ -9339,7 +9374,7 @@
       <c r="BH113" s="7"/>
       <c r="BI113" s="7"/>
     </row>
-    <row r="114" spans="1:61">
+    <row r="114" spans="1:61" x14ac:dyDescent="0.2">
       <c r="C114" s="33"/>
       <c r="F114" s="23"/>
       <c r="G114" s="13"/>
@@ -9401,7 +9436,7 @@
       <c r="BH114" s="7"/>
       <c r="BI114" s="7"/>
     </row>
-    <row r="115" spans="1:61">
+    <row r="115" spans="1:61" x14ac:dyDescent="0.2">
       <c r="F115" s="14"/>
       <c r="G115" s="13"/>
       <c r="H115" s="13"/>
@@ -9462,7 +9497,7 @@
       <c r="BH115" s="7"/>
       <c r="BI115" s="7"/>
     </row>
-    <row r="116" spans="1:61">
+    <row r="116" spans="1:61" x14ac:dyDescent="0.2">
       <c r="F116" s="14"/>
       <c r="G116" s="13"/>
       <c r="H116" s="13"/>
@@ -9523,7 +9558,7 @@
       <c r="BH116" s="7"/>
       <c r="BI116" s="7"/>
     </row>
-    <row r="117" spans="1:61">
+    <row r="117" spans="1:61" x14ac:dyDescent="0.2">
       <c r="F117" s="14"/>
       <c r="G117" s="13"/>
       <c r="H117" s="13"/>
@@ -9584,7 +9619,7 @@
       <c r="BH117" s="7"/>
       <c r="BI117" s="7"/>
     </row>
-    <row r="118" spans="1:61">
+    <row r="118" spans="1:61" x14ac:dyDescent="0.2">
       <c r="F118" s="14"/>
       <c r="G118" s="13"/>
       <c r="H118" s="13"/>
@@ -9645,7 +9680,7 @@
       <c r="BH118" s="7"/>
       <c r="BI118" s="7"/>
     </row>
-    <row r="119" spans="1:61">
+    <row r="119" spans="1:61" x14ac:dyDescent="0.2">
       <c r="F119" s="14"/>
       <c r="G119" s="13"/>
       <c r="H119" s="13"/>
@@ -9706,7 +9741,7 @@
       <c r="BH119" s="7"/>
       <c r="BI119" s="7"/>
     </row>
-    <row r="120" spans="1:61">
+    <row r="120" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A120" s="9"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -9772,7 +9807,7 @@
       <c r="BH120" s="7"/>
       <c r="BI120" s="7"/>
     </row>
-    <row r="121" spans="1:61" ht="13.5" thickBot="1">
+    <row r="121" spans="1:61" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A121" s="9"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -9838,7 +9873,7 @@
       <c r="BH121" s="7"/>
       <c r="BI121" s="7"/>
     </row>
-    <row r="122" spans="1:61" s="5" customFormat="1" ht="13.5" thickBot="1">
+    <row r="122" spans="1:61" s="5" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A122" s="9"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -9910,7 +9945,7 @@
       <c r="BH122" s="7"/>
       <c r="BI122" s="7"/>
     </row>
-    <row r="123" spans="1:61">
+    <row r="123" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A123" s="9"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -9973,7 +10008,7 @@
       <c r="BH123" s="7"/>
       <c r="BI123" s="7"/>
     </row>
-    <row r="124" spans="1:61">
+    <row r="124" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A124" s="9"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -9999,7 +10034,7 @@
       <c r="W124" s="7"/>
       <c r="X124" s="7"/>
     </row>
-    <row r="125" spans="1:61">
+    <row r="125" spans="1:61" x14ac:dyDescent="0.2">
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
       <c r="H125" s="7"/>
@@ -10020,7 +10055,7 @@
       <c r="W125" s="7"/>
       <c r="X125" s="7"/>
     </row>
-    <row r="126" spans="1:61">
+    <row r="126" spans="1:61" x14ac:dyDescent="0.2">
       <c r="F126" s="7"/>
       <c r="G126" s="7"/>
       <c r="H126" s="7"/>
@@ -10041,7 +10076,7 @@
       <c r="W126" s="7"/>
       <c r="X126" s="7"/>
     </row>
-    <row r="127" spans="1:61">
+    <row r="127" spans="1:61" x14ac:dyDescent="0.2">
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
       <c r="H127" s="7"/>
@@ -10062,7 +10097,7 @@
       <c r="W127" s="7"/>
       <c r="X127" s="7"/>
     </row>
-    <row r="128" spans="1:61">
+    <row r="128" spans="1:61" x14ac:dyDescent="0.2">
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
       <c r="H128" s="7"/>
@@ -10083,7 +10118,7 @@
       <c r="W128" s="7"/>
       <c r="X128" s="7"/>
     </row>
-    <row r="129" spans="6:24">
+    <row r="129" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F129" s="7"/>
       <c r="G129" s="7"/>
       <c r="H129" s="7"/>
@@ -10104,7 +10139,7 @@
       <c r="W129" s="7"/>
       <c r="X129" s="7"/>
     </row>
-    <row r="130" spans="6:24">
+    <row r="130" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F130" s="7"/>
       <c r="G130" s="7"/>
       <c r="H130" s="7"/>
@@ -10125,7 +10160,7 @@
       <c r="W130" s="7"/>
       <c r="X130" s="7"/>
     </row>
-    <row r="131" spans="6:24">
+    <row r="131" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
       <c r="H131" s="7"/>
@@ -10143,7 +10178,7 @@
       <c r="T131" s="7"/>
       <c r="U131" s="7"/>
     </row>
-    <row r="132" spans="6:24">
+    <row r="132" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
       <c r="H132" s="7"/>
@@ -10161,7 +10196,7 @@
       <c r="T132" s="7"/>
       <c r="U132" s="7"/>
     </row>
-    <row r="133" spans="6:24">
+    <row r="133" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F133" s="7"/>
       <c r="G133" s="7"/>
       <c r="H133" s="7"/>
@@ -10179,7 +10214,7 @@
       <c r="T133" s="7"/>
       <c r="U133" s="7"/>
     </row>
-    <row r="134" spans="6:24">
+    <row r="134" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F134" s="7"/>
       <c r="G134" s="7"/>
       <c r="H134" s="7"/>
@@ -10197,7 +10232,7 @@
       <c r="T134" s="7"/>
       <c r="U134" s="7"/>
     </row>
-    <row r="135" spans="6:24">
+    <row r="135" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
       <c r="H135" s="7"/>
@@ -10215,7 +10250,7 @@
       <c r="T135" s="7"/>
       <c r="U135" s="7"/>
     </row>
-    <row r="136" spans="6:24">
+    <row r="136" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F136" s="7"/>
       <c r="G136" s="7"/>
       <c r="H136" s="7"/>
@@ -10233,7 +10268,7 @@
       <c r="T136" s="7"/>
       <c r="U136" s="7"/>
     </row>
-    <row r="137" spans="6:24">
+    <row r="137" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
       <c r="H137" s="7"/>
@@ -10251,7 +10286,7 @@
       <c r="T137" s="7"/>
       <c r="U137" s="7"/>
     </row>
-    <row r="138" spans="6:24">
+    <row r="138" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F138" s="7"/>
       <c r="G138" s="7"/>
       <c r="H138" s="7"/>
@@ -10269,7 +10304,7 @@
       <c r="T138" s="7"/>
       <c r="U138" s="7"/>
     </row>
-    <row r="139" spans="6:24">
+    <row r="139" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F139" s="7"/>
       <c r="G139" s="7"/>
       <c r="H139" s="7"/>
@@ -10287,119 +10322,119 @@
       <c r="T139" s="7"/>
       <c r="U139" s="7"/>
     </row>
-    <row r="140" spans="6:24">
+    <row r="140" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F140" s="7"/>
       <c r="G140" s="7"/>
       <c r="H140" s="7"/>
       <c r="I140" s="19"/>
       <c r="J140" s="19"/>
     </row>
-    <row r="141" spans="6:24">
+    <row r="141" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F141" s="7"/>
       <c r="G141" s="7"/>
       <c r="H141" s="7"/>
       <c r="I141" s="19"/>
       <c r="J141" s="19"/>
     </row>
-    <row r="142" spans="6:24">
+    <row r="142" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F142" s="7"/>
       <c r="G142" s="7"/>
       <c r="H142" s="7"/>
       <c r="I142" s="19"/>
       <c r="J142" s="19"/>
     </row>
-    <row r="143" spans="6:24">
+    <row r="143" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F143" s="7"/>
       <c r="G143" s="7"/>
       <c r="H143" s="7"/>
       <c r="I143" s="19"/>
       <c r="J143" s="19"/>
     </row>
-    <row r="144" spans="6:24">
+    <row r="144" spans="6:24" x14ac:dyDescent="0.2">
       <c r="F144" s="7"/>
       <c r="G144" s="7"/>
       <c r="H144" s="7"/>
       <c r="I144" s="19"/>
       <c r="J144" s="19"/>
     </row>
-    <row r="145" spans="5:13">
+    <row r="145" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F145" s="7"/>
       <c r="G145" s="7"/>
       <c r="H145" s="7"/>
       <c r="I145" s="19"/>
       <c r="J145" s="19"/>
     </row>
-    <row r="146" spans="5:13">
+    <row r="146" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F146" s="7"/>
       <c r="G146" s="7"/>
       <c r="H146" s="7"/>
       <c r="I146" s="19"/>
       <c r="J146" s="19"/>
     </row>
-    <row r="147" spans="5:13">
+    <row r="147" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F147" s="7"/>
       <c r="G147" s="7"/>
       <c r="H147" s="7"/>
       <c r="I147" s="19"/>
       <c r="J147" s="19"/>
     </row>
-    <row r="148" spans="5:13">
+    <row r="148" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F148" s="7"/>
       <c r="G148" s="7"/>
       <c r="H148" s="7"/>
       <c r="I148" s="19"/>
       <c r="J148" s="19"/>
     </row>
-    <row r="149" spans="5:13">
+    <row r="149" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F149" s="7"/>
       <c r="G149" s="7"/>
       <c r="H149" s="7"/>
       <c r="I149" s="19"/>
       <c r="J149" s="19"/>
     </row>
-    <row r="150" spans="5:13">
+    <row r="150" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F150" s="7"/>
       <c r="G150" s="7"/>
       <c r="H150" s="7"/>
       <c r="I150" s="19"/>
       <c r="J150" s="19"/>
     </row>
-    <row r="151" spans="5:13">
+    <row r="151" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F151" s="7"/>
       <c r="G151" s="7"/>
       <c r="H151" s="7"/>
       <c r="I151" s="19"/>
       <c r="J151" s="19"/>
     </row>
-    <row r="152" spans="5:13">
+    <row r="152" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F152" s="7"/>
       <c r="G152" s="7"/>
       <c r="H152" s="7"/>
       <c r="I152" s="19"/>
       <c r="J152" s="19"/>
     </row>
-    <row r="153" spans="5:13">
+    <row r="153" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
       <c r="H153" s="7"/>
       <c r="I153" s="19"/>
       <c r="J153" s="19"/>
     </row>
-    <row r="154" spans="5:13">
+    <row r="154" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F154" s="7"/>
       <c r="G154" s="7"/>
       <c r="H154" s="7"/>
       <c r="I154" s="19"/>
       <c r="J154" s="19"/>
     </row>
-    <row r="155" spans="5:13">
+    <row r="155" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F155" s="7"/>
       <c r="G155" s="7"/>
       <c r="H155" s="7"/>
       <c r="I155" s="19"/>
       <c r="J155" s="19"/>
     </row>
-    <row r="156" spans="5:13">
+    <row r="156" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F156" s="155"/>
       <c r="G156" s="155"/>
       <c r="H156" s="7"/>
@@ -10409,7 +10444,7 @@
       <c r="L156" s="43"/>
       <c r="M156" s="5"/>
     </row>
-    <row r="157" spans="5:13">
+    <row r="157" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E157" s="7"/>
       <c r="F157" s="7"/>
       <c r="G157" s="7"/>
@@ -10417,7 +10452,7 @@
       <c r="I157" s="19"/>
       <c r="J157" s="19"/>
     </row>
-    <row r="158" spans="5:13">
+    <row r="158" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E158" s="7"/>
       <c r="F158" s="7"/>
       <c r="G158" s="7"/>
@@ -10425,7 +10460,7 @@
       <c r="I158" s="19"/>
       <c r="J158" s="19"/>
     </row>
-    <row r="159" spans="5:13">
+    <row r="159" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E159" s="7"/>
       <c r="F159" s="7"/>
       <c r="G159" s="7"/>
@@ -10433,7 +10468,7 @@
       <c r="I159" s="19"/>
       <c r="J159" s="19"/>
     </row>
-    <row r="160" spans="5:13">
+    <row r="160" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E160" s="7"/>
       <c r="F160" s="7"/>
       <c r="G160" s="7"/>
@@ -10441,7 +10476,7 @@
       <c r="I160" s="19"/>
       <c r="J160" s="19"/>
     </row>
-    <row r="161" spans="5:10">
+    <row r="161" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E161" s="7"/>
       <c r="F161" s="7"/>
       <c r="G161" s="7"/>
@@ -10449,7 +10484,7 @@
       <c r="I161" s="19"/>
       <c r="J161" s="19"/>
     </row>
-    <row r="162" spans="5:10">
+    <row r="162" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E162" s="7"/>
       <c r="F162" s="7"/>
       <c r="G162" s="7"/>
@@ -10457,7 +10492,7 @@
       <c r="I162" s="19"/>
       <c r="J162" s="19"/>
     </row>
-    <row r="163" spans="5:10">
+    <row r="163" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E163" s="7"/>
       <c r="F163" s="7"/>
       <c r="G163" s="7"/>
@@ -10465,7 +10500,7 @@
       <c r="I163" s="19"/>
       <c r="J163" s="19"/>
     </row>
-    <row r="164" spans="5:10">
+    <row r="164" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E164" s="7"/>
       <c r="F164" s="7"/>
       <c r="G164" s="7"/>
@@ -10473,7 +10508,7 @@
       <c r="I164" s="19"/>
       <c r="J164" s="19"/>
     </row>
-    <row r="165" spans="5:10">
+    <row r="165" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E165" s="7"/>
       <c r="F165" s="7"/>
       <c r="G165" s="7"/>
@@ -10481,7 +10516,7 @@
       <c r="I165" s="19"/>
       <c r="J165" s="19"/>
     </row>
-    <row r="166" spans="5:10">
+    <row r="166" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E166" s="7"/>
       <c r="F166" s="7"/>
       <c r="G166" s="7"/>
@@ -10489,7 +10524,7 @@
       <c r="I166" s="19"/>
       <c r="J166" s="19"/>
     </row>
-    <row r="167" spans="5:10">
+    <row r="167" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E167" s="7"/>
       <c r="F167" s="7"/>
       <c r="G167" s="7"/>
@@ -10497,7 +10532,7 @@
       <c r="I167" s="19"/>
       <c r="J167" s="19"/>
     </row>
-    <row r="168" spans="5:10">
+    <row r="168" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E168" s="7"/>
       <c r="F168" s="7"/>
       <c r="G168" s="7"/>
@@ -10505,7 +10540,7 @@
       <c r="I168" s="19"/>
       <c r="J168" s="19"/>
     </row>
-    <row r="169" spans="5:10">
+    <row r="169" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E169" s="7"/>
       <c r="F169" s="7"/>
       <c r="G169" s="7"/>
@@ -10513,7 +10548,7 @@
       <c r="I169" s="19"/>
       <c r="J169" s="19"/>
     </row>
-    <row r="170" spans="5:10">
+    <row r="170" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E170" s="7"/>
       <c r="F170" s="7"/>
       <c r="G170" s="7"/>
@@ -10521,7 +10556,7 @@
       <c r="I170" s="19"/>
       <c r="J170" s="19"/>
     </row>
-    <row r="171" spans="5:10">
+    <row r="171" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E171" s="7"/>
       <c r="F171" s="7"/>
       <c r="G171" s="7"/>
@@ -10529,7 +10564,7 @@
       <c r="I171" s="19"/>
       <c r="J171" s="19"/>
     </row>
-    <row r="172" spans="5:10">
+    <row r="172" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E172" s="7"/>
       <c r="F172" s="7"/>
       <c r="G172" s="7"/>
@@ -10537,7 +10572,7 @@
       <c r="I172" s="19"/>
       <c r="J172" s="19"/>
     </row>
-    <row r="173" spans="5:10">
+    <row r="173" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E173" s="7"/>
       <c r="F173" s="7"/>
       <c r="G173" s="7"/>
@@ -10545,7 +10580,7 @@
       <c r="I173" s="19"/>
       <c r="J173" s="19"/>
     </row>
-    <row r="174" spans="5:10">
+    <row r="174" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E174" s="7"/>
       <c r="F174" s="7"/>
       <c r="G174" s="7"/>
@@ -10553,7 +10588,7 @@
       <c r="I174" s="19"/>
       <c r="J174" s="19"/>
     </row>
-    <row r="175" spans="5:10">
+    <row r="175" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E175" s="7"/>
       <c r="F175" s="7"/>
       <c r="G175" s="7"/>
@@ -10561,7 +10596,7 @@
       <c r="I175" s="19"/>
       <c r="J175" s="19"/>
     </row>
-    <row r="176" spans="5:10">
+    <row r="176" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E176" s="7"/>
       <c r="F176" s="7"/>
       <c r="G176" s="7"/>
@@ -10569,7 +10604,7 @@
       <c r="I176" s="19"/>
       <c r="J176" s="19"/>
     </row>
-    <row r="177" spans="5:10">
+    <row r="177" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E177" s="7"/>
       <c r="F177" s="7"/>
       <c r="G177" s="7"/>
@@ -10577,7 +10612,7 @@
       <c r="I177" s="19"/>
       <c r="J177" s="19"/>
     </row>
-    <row r="178" spans="5:10">
+    <row r="178" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E178" s="7"/>
       <c r="F178" s="7"/>
       <c r="G178" s="7"/>
@@ -10585,7 +10620,7 @@
       <c r="I178" s="19"/>
       <c r="J178" s="19"/>
     </row>
-    <row r="179" spans="5:10">
+    <row r="179" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E179" s="7"/>
       <c r="F179" s="7"/>
       <c r="G179" s="7"/>
@@ -10593,7 +10628,7 @@
       <c r="I179" s="19"/>
       <c r="J179" s="19"/>
     </row>
-    <row r="180" spans="5:10">
+    <row r="180" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E180" s="7"/>
       <c r="F180" s="7"/>
       <c r="G180" s="7"/>
@@ -10601,7 +10636,7 @@
       <c r="I180" s="19"/>
       <c r="J180" s="19"/>
     </row>
-    <row r="181" spans="5:10">
+    <row r="181" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E181" s="7"/>
       <c r="F181" s="7"/>
       <c r="G181" s="7"/>
@@ -10609,7 +10644,7 @@
       <c r="I181" s="19"/>
       <c r="J181" s="19"/>
     </row>
-    <row r="182" spans="5:10">
+    <row r="182" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E182" s="7"/>
       <c r="F182" s="7"/>
       <c r="G182" s="7"/>
@@ -10617,7 +10652,7 @@
       <c r="I182" s="19"/>
       <c r="J182" s="19"/>
     </row>
-    <row r="183" spans="5:10">
+    <row r="183" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E183" s="7"/>
       <c r="F183" s="7"/>
       <c r="G183" s="7"/>
@@ -10625,7 +10660,7 @@
       <c r="I183" s="19"/>
       <c r="J183" s="19"/>
     </row>
-    <row r="184" spans="5:10">
+    <row r="184" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E184" s="7"/>
       <c r="F184" s="7"/>
       <c r="G184" s="7"/>
@@ -10633,7 +10668,7 @@
       <c r="I184" s="19"/>
       <c r="J184" s="19"/>
     </row>
-    <row r="185" spans="5:10">
+    <row r="185" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E185" s="7"/>
       <c r="F185" s="7"/>
       <c r="G185" s="7"/>
@@ -10641,7 +10676,7 @@
       <c r="I185" s="19"/>
       <c r="J185" s="19"/>
     </row>
-    <row r="186" spans="5:10">
+    <row r="186" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E186" s="7"/>
       <c r="F186" s="7"/>
       <c r="G186" s="7"/>
@@ -10649,7 +10684,7 @@
       <c r="I186" s="19"/>
       <c r="J186" s="19"/>
     </row>
-    <row r="187" spans="5:10">
+    <row r="187" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E187" s="7"/>
       <c r="F187" s="7"/>
       <c r="G187" s="7"/>
@@ -10657,7 +10692,7 @@
       <c r="I187" s="19"/>
       <c r="J187" s="19"/>
     </row>
-    <row r="188" spans="5:10">
+    <row r="188" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E188" s="7"/>
       <c r="F188" s="7"/>
       <c r="G188" s="7"/>
@@ -10665,7 +10700,7 @@
       <c r="I188" s="19"/>
       <c r="J188" s="19"/>
     </row>
-    <row r="189" spans="5:10">
+    <row r="189" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E189" s="7"/>
       <c r="F189" s="7"/>
       <c r="G189" s="7"/>
@@ -10673,7 +10708,7 @@
       <c r="I189" s="19"/>
       <c r="J189" s="19"/>
     </row>
-    <row r="190" spans="5:10">
+    <row r="190" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E190" s="7"/>
       <c r="F190" s="7"/>
       <c r="G190" s="7"/>
@@ -10681,7 +10716,7 @@
       <c r="I190" s="19"/>
       <c r="J190" s="19"/>
     </row>
-    <row r="191" spans="5:10">
+    <row r="191" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E191" s="7"/>
       <c r="F191" s="7"/>
       <c r="G191" s="7"/>
@@ -10689,7 +10724,7 @@
       <c r="I191" s="19"/>
       <c r="J191" s="19"/>
     </row>
-    <row r="192" spans="5:10">
+    <row r="192" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E192" s="7"/>
       <c r="F192" s="7"/>
       <c r="G192" s="7"/>
@@ -10697,7 +10732,7 @@
       <c r="I192" s="19"/>
       <c r="J192" s="19"/>
     </row>
-    <row r="193" spans="5:10">
+    <row r="193" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E193" s="7"/>
       <c r="F193" s="7"/>
       <c r="G193" s="7"/>
@@ -10705,7 +10740,7 @@
       <c r="I193" s="19"/>
       <c r="J193" s="19"/>
     </row>
-    <row r="194" spans="5:10">
+    <row r="194" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E194" s="7"/>
       <c r="F194" s="7"/>
       <c r="G194" s="7"/>
@@ -10713,7 +10748,7 @@
       <c r="I194" s="19"/>
       <c r="J194" s="19"/>
     </row>
-    <row r="195" spans="5:10">
+    <row r="195" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E195" s="7"/>
       <c r="F195" s="7"/>
       <c r="G195" s="7"/>
@@ -10721,7 +10756,7 @@
       <c r="I195" s="19"/>
       <c r="J195" s="19"/>
     </row>
-    <row r="196" spans="5:10">
+    <row r="196" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E196" s="7"/>
       <c r="F196" s="7"/>
       <c r="G196" s="7"/>
@@ -10729,7 +10764,7 @@
       <c r="I196" s="19"/>
       <c r="J196" s="19"/>
     </row>
-    <row r="197" spans="5:10">
+    <row r="197" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E197" s="7"/>
       <c r="F197" s="7"/>
       <c r="G197" s="7"/>
@@ -10737,7 +10772,7 @@
       <c r="I197" s="19"/>
       <c r="J197" s="19"/>
     </row>
-    <row r="198" spans="5:10">
+    <row r="198" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E198" s="7"/>
       <c r="F198" s="7"/>
       <c r="G198" s="7"/>
@@ -10745,7 +10780,7 @@
       <c r="I198" s="19"/>
       <c r="J198" s="19"/>
     </row>
-    <row r="199" spans="5:10">
+    <row r="199" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E199" s="7"/>
       <c r="F199" s="7"/>
       <c r="G199" s="7"/>
@@ -10753,7 +10788,7 @@
       <c r="I199" s="19"/>
       <c r="J199" s="19"/>
     </row>
-    <row r="200" spans="5:10">
+    <row r="200" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E200" s="7"/>
       <c r="F200" s="7"/>
       <c r="G200" s="7"/>
@@ -10761,7 +10796,7 @@
       <c r="I200" s="19"/>
       <c r="J200" s="19"/>
     </row>
-    <row r="201" spans="5:10">
+    <row r="201" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E201" s="7"/>
       <c r="F201" s="7"/>
       <c r="G201" s="7"/>
@@ -10769,7 +10804,7 @@
       <c r="I201" s="19"/>
       <c r="J201" s="19"/>
     </row>
-    <row r="202" spans="5:10">
+    <row r="202" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E202" s="7"/>
       <c r="F202" s="7"/>
       <c r="G202" s="7"/>
@@ -10777,7 +10812,7 @@
       <c r="I202" s="19"/>
       <c r="J202" s="19"/>
     </row>
-    <row r="203" spans="5:10">
+    <row r="203" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E203" s="7"/>
       <c r="F203" s="7"/>
       <c r="G203" s="7"/>
@@ -10785,7 +10820,7 @@
       <c r="I203" s="19"/>
       <c r="J203" s="19"/>
     </row>
-    <row r="204" spans="5:10">
+    <row r="204" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E204" s="7"/>
       <c r="F204" s="7"/>
       <c r="G204" s="7"/>
@@ -10793,7 +10828,7 @@
       <c r="I204" s="19"/>
       <c r="J204" s="19"/>
     </row>
-    <row r="205" spans="5:10">
+    <row r="205" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E205" s="7"/>
       <c r="F205" s="7"/>
       <c r="G205" s="7"/>
@@ -10801,7 +10836,7 @@
       <c r="I205" s="19"/>
       <c r="J205" s="19"/>
     </row>
-    <row r="206" spans="5:10">
+    <row r="206" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E206" s="7"/>
       <c r="F206" s="7"/>
       <c r="G206" s="7"/>
@@ -10809,7 +10844,7 @@
       <c r="I206" s="19"/>
       <c r="J206" s="19"/>
     </row>
-    <row r="207" spans="5:10">
+    <row r="207" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E207" s="7"/>
       <c r="F207" s="7"/>
       <c r="G207" s="7"/>
@@ -10817,7 +10852,7 @@
       <c r="I207" s="19"/>
       <c r="J207" s="19"/>
     </row>
-    <row r="208" spans="5:10">
+    <row r="208" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E208" s="7"/>
       <c r="F208" s="7"/>
       <c r="G208" s="7"/>
@@ -10825,7 +10860,7 @@
       <c r="I208" s="19"/>
       <c r="J208" s="19"/>
     </row>
-    <row r="209" spans="5:10">
+    <row r="209" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E209" s="7"/>
       <c r="F209" s="7"/>
       <c r="G209" s="7"/>
@@ -10833,7 +10868,7 @@
       <c r="I209" s="19"/>
       <c r="J209" s="19"/>
     </row>
-    <row r="210" spans="5:10">
+    <row r="210" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E210" s="7"/>
       <c r="F210" s="7"/>
       <c r="G210" s="7"/>
@@ -10841,7 +10876,7 @@
       <c r="I210" s="19"/>
       <c r="J210" s="19"/>
     </row>
-    <row r="211" spans="5:10">
+    <row r="211" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E211" s="7"/>
       <c r="F211" s="7"/>
       <c r="G211" s="7"/>
@@ -10849,7 +10884,7 @@
       <c r="I211" s="19"/>
       <c r="J211" s="19"/>
     </row>
-    <row r="212" spans="5:10">
+    <row r="212" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E212" s="7"/>
       <c r="F212" s="7"/>
       <c r="G212" s="7"/>
@@ -10857,7 +10892,7 @@
       <c r="I212" s="19"/>
       <c r="J212" s="19"/>
     </row>
-    <row r="213" spans="5:10">
+    <row r="213" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E213" s="7"/>
       <c r="F213" s="7"/>
       <c r="G213" s="7"/>
@@ -10865,7 +10900,7 @@
       <c r="I213" s="19"/>
       <c r="J213" s="19"/>
     </row>
-    <row r="214" spans="5:10">
+    <row r="214" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E214" s="7"/>
       <c r="F214" s="7"/>
       <c r="G214" s="7"/>
@@ -10873,7 +10908,7 @@
       <c r="I214" s="19"/>
       <c r="J214" s="19"/>
     </row>
-    <row r="215" spans="5:10">
+    <row r="215" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E215" s="7"/>
       <c r="F215" s="7"/>
       <c r="G215" s="7"/>
@@ -10881,7 +10916,7 @@
       <c r="I215" s="19"/>
       <c r="J215" s="19"/>
     </row>
-    <row r="216" spans="5:10">
+    <row r="216" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E216" s="7"/>
       <c r="F216" s="7"/>
       <c r="G216" s="7"/>
@@ -10889,7 +10924,7 @@
       <c r="I216" s="19"/>
       <c r="J216" s="19"/>
     </row>
-    <row r="217" spans="5:10">
+    <row r="217" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E217" s="7"/>
       <c r="F217" s="7"/>
       <c r="G217" s="7"/>
@@ -10897,7 +10932,7 @@
       <c r="I217" s="19"/>
       <c r="J217" s="19"/>
     </row>
-    <row r="218" spans="5:10">
+    <row r="218" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E218" s="7"/>
       <c r="F218" s="7"/>
       <c r="G218" s="7"/>
@@ -10905,7 +10940,7 @@
       <c r="I218" s="19"/>
       <c r="J218" s="19"/>
     </row>
-    <row r="219" spans="5:10">
+    <row r="219" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E219" s="7"/>
       <c r="F219" s="7"/>
       <c r="G219" s="7"/>
@@ -10913,7 +10948,7 @@
       <c r="I219" s="19"/>
       <c r="J219" s="19"/>
     </row>
-    <row r="220" spans="5:10">
+    <row r="220" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E220" s="7"/>
       <c r="F220" s="7"/>
       <c r="G220" s="7"/>
@@ -10921,7 +10956,7 @@
       <c r="I220" s="19"/>
       <c r="J220" s="19"/>
     </row>
-    <row r="221" spans="5:10">
+    <row r="221" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E221" s="7"/>
       <c r="F221" s="7"/>
       <c r="G221" s="7"/>
@@ -10929,7 +10964,7 @@
       <c r="I221" s="19"/>
       <c r="J221" s="19"/>
     </row>
-    <row r="222" spans="5:10">
+    <row r="222" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E222" s="7"/>
       <c r="F222" s="7"/>
       <c r="G222" s="7"/>
@@ -10937,7 +10972,7 @@
       <c r="I222" s="19"/>
       <c r="J222" s="19"/>
     </row>
-    <row r="223" spans="5:10">
+    <row r="223" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E223" s="7"/>
       <c r="F223" s="7"/>
       <c r="G223" s="7"/>
@@ -10945,7 +10980,7 @@
       <c r="I223" s="19"/>
       <c r="J223" s="19"/>
     </row>
-    <row r="224" spans="5:10">
+    <row r="224" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E224" s="7"/>
       <c r="F224" s="7"/>
       <c r="G224" s="7"/>
@@ -10953,7 +10988,7 @@
       <c r="I224" s="19"/>
       <c r="J224" s="19"/>
     </row>
-    <row r="225" spans="5:10">
+    <row r="225" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E225" s="7"/>
       <c r="F225" s="7"/>
       <c r="G225" s="7"/>
@@ -10961,7 +10996,7 @@
       <c r="I225" s="19"/>
       <c r="J225" s="19"/>
     </row>
-    <row r="226" spans="5:10">
+    <row r="226" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E226" s="7"/>
       <c r="F226" s="7"/>
       <c r="G226" s="7"/>
@@ -10969,7 +11004,7 @@
       <c r="I226" s="19"/>
       <c r="J226" s="19"/>
     </row>
-    <row r="227" spans="5:10">
+    <row r="227" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E227" s="7"/>
       <c r="F227" s="7"/>
       <c r="G227" s="7"/>
@@ -10977,7 +11012,7 @@
       <c r="I227" s="19"/>
       <c r="J227" s="19"/>
     </row>
-    <row r="228" spans="5:10">
+    <row r="228" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E228" s="7"/>
       <c r="F228" s="7"/>
       <c r="G228" s="7"/>
@@ -10985,7 +11020,7 @@
       <c r="I228" s="19"/>
       <c r="J228" s="19"/>
     </row>
-    <row r="229" spans="5:10">
+    <row r="229" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E229" s="7"/>
       <c r="F229" s="7"/>
       <c r="G229" s="7"/>
@@ -10993,7 +11028,7 @@
       <c r="I229" s="19"/>
       <c r="J229" s="19"/>
     </row>
-    <row r="230" spans="5:10">
+    <row r="230" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E230" s="7"/>
       <c r="F230" s="7"/>
       <c r="G230" s="7"/>
@@ -11001,7 +11036,7 @@
       <c r="I230" s="19"/>
       <c r="J230" s="19"/>
     </row>
-    <row r="231" spans="5:10">
+    <row r="231" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E231" s="7"/>
       <c r="F231" s="7"/>
       <c r="G231" s="7"/>
@@ -11009,7 +11044,7 @@
       <c r="I231" s="19"/>
       <c r="J231" s="19"/>
     </row>
-    <row r="232" spans="5:10">
+    <row r="232" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E232" s="7"/>
       <c r="F232" s="7"/>
       <c r="G232" s="7"/>

</xml_diff>